<commit_message>
atualizacao ate 16 de agosto
</commit_message>
<xml_diff>
--- a/Sistema-Operacional/Monitoramento - Mananciais Críticos.xlsx
+++ b/Sistema-Operacional/Monitoramento - Mananciais Críticos.xlsx
@@ -28,10 +28,10 @@
     <t>AN_TRI_202008</t>
   </si>
   <si>
-    <t>AC_20200807</t>
-  </si>
-  <si>
-    <t>AN_20200807</t>
+    <t>AC_20200816</t>
+  </si>
+  <si>
+    <t>AN_20200816</t>
   </si>
   <si>
     <t>SPI1_202007</t>
@@ -52,7 +52,7 @@
     <t>AN_COTA_202007</t>
   </si>
   <si>
-    <t>AN_COTA_20200807</t>
+    <t>AN_COTA_20200816</t>
   </si>
   <si>
     <t>SIA</t>
@@ -591,19 +591,19 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>-29</v>
+        <v>-26.2</v>
       </c>
       <c r="D2">
-        <v>-40.7</v>
+        <v>-33</v>
       </c>
       <c r="E2">
-        <v>-43.1</v>
+        <v>-24.2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G2">
-        <v>-100</v>
+        <v>-27.2</v>
       </c>
       <c r="H2">
         <v>-1.14</v>
@@ -624,7 +624,7 @@
         <v>-10.64</v>
       </c>
       <c r="N2">
-        <v>-10.66</v>
+        <v>-10.78</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -635,19 +635,19 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>-36.1</v>
+        <v>-31.1</v>
       </c>
       <c r="D3">
-        <v>-55.6</v>
+        <v>-43</v>
       </c>
       <c r="E3">
-        <v>-34.2</v>
+        <v>-8.1</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>63.5</v>
       </c>
       <c r="G3">
-        <v>-99.8</v>
+        <v>44.6</v>
       </c>
       <c r="H3">
         <v>-1.1</v>
@@ -668,7 +668,7 @@
         <v>-50.72</v>
       </c>
       <c r="N3">
-        <v>-45.41</v>
+        <v>-46.38</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -679,19 +679,19 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>-39.5</v>
+        <v>-36.9</v>
       </c>
       <c r="D4">
-        <v>-47.5</v>
+        <v>-41.2</v>
       </c>
       <c r="E4">
-        <v>-36.8</v>
+        <v>-22</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="G4">
-        <v>-100</v>
+        <v>-40.4</v>
       </c>
       <c r="H4">
         <v>-1.14</v>
@@ -714,19 +714,19 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>-16.3</v>
+        <v>-10.4</v>
       </c>
       <c r="D5">
-        <v>-19.8</v>
+        <v>-6.1</v>
       </c>
       <c r="E5">
-        <v>-33.7</v>
+        <v>-0.3</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>84.3</v>
       </c>
       <c r="G5">
-        <v>-100</v>
+        <v>33.6</v>
       </c>
       <c r="H5">
         <v>-0.52</v>
@@ -758,19 +758,19 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>-30</v>
+        <v>-24.9</v>
       </c>
       <c r="D6">
-        <v>-44.7</v>
+        <v>-32.3</v>
       </c>
       <c r="E6">
-        <v>-59.9</v>
+        <v>-32.3</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="G6">
-        <v>-100</v>
+        <v>-6.1</v>
       </c>
       <c r="H6">
         <v>-0.91</v>
@@ -791,7 +791,7 @@
         <v>-13.2</v>
       </c>
       <c r="N6">
-        <v>-14.94</v>
+        <v>-12.87</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -802,19 +802,19 @@
         <v>19</v>
       </c>
       <c r="C7">
-        <v>-26.4</v>
+        <v>-20.8</v>
       </c>
       <c r="D7">
-        <v>-40.4</v>
+        <v>-27.4</v>
       </c>
       <c r="E7">
-        <v>-52.3</v>
+        <v>-20.6</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>90.7</v>
       </c>
       <c r="G7">
-        <v>-100</v>
+        <v>-5.7</v>
       </c>
       <c r="H7">
         <v>-0.47</v>
@@ -837,19 +837,19 @@
         <v>20</v>
       </c>
       <c r="C8">
-        <v>-59.1</v>
+        <v>-54.3</v>
       </c>
       <c r="D8">
-        <v>-61.8</v>
+        <v>-49.8</v>
       </c>
       <c r="E8">
-        <v>-45.3</v>
+        <v>-20.5</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>73.3</v>
       </c>
       <c r="G8">
-        <v>-100</v>
+        <v>-12.9</v>
       </c>
       <c r="H8">
         <v>-1.39</v>
@@ -881,19 +881,19 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>-32.8</v>
+        <v>-29.1</v>
       </c>
       <c r="D9">
-        <v>-40.5</v>
+        <v>-32</v>
       </c>
       <c r="E9">
-        <v>-50.3</v>
+        <v>-32.4</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
+        <v>66.7</v>
       </c>
       <c r="G9">
-        <v>-99.90000000000001</v>
+        <v>-26</v>
       </c>
       <c r="H9">
         <v>-0.68</v>
@@ -916,19 +916,19 @@
         <v>22</v>
       </c>
       <c r="C10">
-        <v>-54.5</v>
+        <v>-50</v>
       </c>
       <c r="D10">
-        <v>-69.09999999999999</v>
+        <v>-58.5</v>
       </c>
       <c r="E10">
-        <v>-60.2</v>
+        <v>-38.1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>65.2</v>
       </c>
       <c r="G10">
-        <v>-100</v>
+        <v>-15.7</v>
       </c>
       <c r="H10">
         <v>-1.03</v>
@@ -949,7 +949,7 @@
         <v>-38.28</v>
       </c>
       <c r="N10">
-        <v>-43.58</v>
+        <v>-28.1</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -960,19 +960,19 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>-49.4</v>
+        <v>-46.1</v>
       </c>
       <c r="D11">
-        <v>-61.3</v>
+        <v>-52.8</v>
       </c>
       <c r="E11">
-        <v>-46.7</v>
+        <v>-29</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>54</v>
       </c>
       <c r="G11">
-        <v>-99.90000000000001</v>
+        <v>-36.3</v>
       </c>
       <c r="H11">
         <v>-0.67</v>
@@ -993,7 +993,7 @@
         <v>-30.45</v>
       </c>
       <c r="N11">
-        <v>-12.7</v>
+        <v>-15.87</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1004,19 +1004,19 @@
         <v>24</v>
       </c>
       <c r="C12">
-        <v>-49.5</v>
+        <v>-46.3</v>
       </c>
       <c r="D12">
-        <v>-61.9</v>
+        <v>-53.6</v>
       </c>
       <c r="E12">
-        <v>-46.6</v>
+        <v>-29.4</v>
       </c>
       <c r="F12">
-        <v>0.1</v>
+        <v>54.6</v>
       </c>
       <c r="G12">
-        <v>-99.90000000000001</v>
+        <v>-37.1</v>
       </c>
       <c r="H12">
         <v>-0.64</v>
@@ -1037,7 +1037,7 @@
         <v>-30.45</v>
       </c>
       <c r="N12">
-        <v>-12.7</v>
+        <v>-15.87</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1048,19 +1048,19 @@
         <v>25</v>
       </c>
       <c r="C13">
-        <v>-28.6</v>
+        <v>-25.2</v>
       </c>
       <c r="D13">
-        <v>-38.6</v>
+        <v>-31.2</v>
       </c>
       <c r="E13">
-        <v>-47.3</v>
+        <v>-31</v>
       </c>
       <c r="F13">
-        <v>0.1</v>
+        <v>62.5</v>
       </c>
       <c r="G13">
-        <v>-99.90000000000001</v>
+        <v>-36</v>
       </c>
       <c r="H13">
         <v>-0.95</v>
@@ -1083,19 +1083,19 @@
         <v>26</v>
       </c>
       <c r="C14">
-        <v>-54.4</v>
+        <v>-51.5</v>
       </c>
       <c r="D14">
-        <v>-65</v>
+        <v>-58.2</v>
       </c>
       <c r="E14">
-        <v>-41.1</v>
+        <v>-25.7</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="G14">
-        <v>-100</v>
+        <v>-35.1</v>
       </c>
       <c r="H14">
         <v>-0.5</v>
@@ -1116,7 +1116,7 @@
         <v>-21.07</v>
       </c>
       <c r="N14">
-        <v>-10.68</v>
+        <v>-11.59</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1127,19 +1127,19 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>-25.9</v>
+        <v>-21.9</v>
       </c>
       <c r="D15">
-        <v>-31.3</v>
+        <v>-21.6</v>
       </c>
       <c r="E15">
-        <v>-14</v>
+        <v>10.4</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="G15">
-        <v>-100</v>
+        <v>-26</v>
       </c>
       <c r="H15">
         <v>-0.64</v>
@@ -1160,7 +1160,7 @@
         <v>-4.67</v>
       </c>
       <c r="N15">
-        <v>-18.99</v>
+        <v>-14.64</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1171,19 +1171,19 @@
         <v>27</v>
       </c>
       <c r="C16">
-        <v>-22.1</v>
+        <v>-17.3</v>
       </c>
       <c r="D16">
-        <v>-20.9</v>
+        <v>-9.5</v>
       </c>
       <c r="E16">
-        <v>-9.4</v>
+        <v>21.1</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="G16">
-        <v>-100</v>
+        <v>-17.2</v>
       </c>
       <c r="H16">
         <v>-0.68</v>
@@ -1204,7 +1204,7 @@
         <v>4.66</v>
       </c>
       <c r="N16">
-        <v>-7.54</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1215,19 +1215,19 @@
         <v>28</v>
       </c>
       <c r="C17">
-        <v>-50.9</v>
+        <v>-48.6</v>
       </c>
       <c r="D17">
-        <v>-52.9</v>
+        <v>-46.3</v>
       </c>
       <c r="E17">
-        <v>-33.9</v>
+        <v>-19</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>43.5</v>
       </c>
       <c r="G17">
-        <v>-100</v>
+        <v>-51.1</v>
       </c>
       <c r="H17">
         <v>-1.3</v>
@@ -1250,19 +1250,19 @@
         <v>29</v>
       </c>
       <c r="C18">
-        <v>-42.4</v>
+        <v>-39.6</v>
       </c>
       <c r="D18">
-        <v>-50.1</v>
+        <v>-42.5</v>
       </c>
       <c r="E18">
-        <v>-53.6</v>
+        <v>-34.4</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="G18">
-        <v>-100</v>
+        <v>-34.2</v>
       </c>
       <c r="H18">
         <v>-1.14</v>
@@ -1283,7 +1283,7 @@
         <v>-10.64</v>
       </c>
       <c r="N18">
-        <v>-10.66</v>
+        <v>-10.78</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1294,19 +1294,19 @@
         <v>30</v>
       </c>
       <c r="C19">
-        <v>-33.4</v>
+        <v>-29.1</v>
       </c>
       <c r="D19">
-        <v>-33.5</v>
+        <v>-22</v>
       </c>
       <c r="E19">
-        <v>-35</v>
+        <v>-5.8</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="G19">
-        <v>-100</v>
+        <v>-25.4</v>
       </c>
       <c r="H19">
         <v>-1.73</v>
@@ -1329,19 +1329,19 @@
         <v>31</v>
       </c>
       <c r="C20">
-        <v>-43.1</v>
+        <v>-40.7</v>
       </c>
       <c r="D20">
-        <v>-50.7</v>
+        <v>-44.6</v>
       </c>
       <c r="E20">
-        <v>-43.7</v>
+        <v>-29</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>47.2</v>
       </c>
       <c r="G20">
-        <v>-100</v>
+        <v>-44.2</v>
       </c>
       <c r="H20">
         <v>-1.06</v>
@@ -1364,19 +1364,19 @@
         <v>32</v>
       </c>
       <c r="C21">
-        <v>-22.7</v>
+        <v>-17.9</v>
       </c>
       <c r="D21">
-        <v>-18.5</v>
+        <v>-6.9</v>
       </c>
       <c r="E21">
-        <v>-5.5</v>
+        <v>25.6</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="G21">
-        <v>-100</v>
+        <v>-21</v>
       </c>
       <c r="H21">
         <v>-0.59</v>
@@ -1405,19 +1405,19 @@
         <v>33</v>
       </c>
       <c r="C22">
-        <v>-35.5</v>
+        <v>-29.2</v>
       </c>
       <c r="D22">
-        <v>-36</v>
+        <v>-20</v>
       </c>
       <c r="E22">
-        <v>-26.8</v>
+        <v>14.6</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>119.4</v>
       </c>
       <c r="G22">
-        <v>-100</v>
+        <v>19.5</v>
       </c>
       <c r="H22">
         <v>-1.11</v>
@@ -1440,19 +1440,19 @@
         <v>34</v>
       </c>
       <c r="C23">
-        <v>-31.2</v>
+        <v>-26.7</v>
       </c>
       <c r="D23">
-        <v>-41.6</v>
+        <v>-31.1</v>
       </c>
       <c r="E23">
-        <v>-54.9</v>
+        <v>-29.2</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>76.5</v>
       </c>
       <c r="G23">
-        <v>-100</v>
+        <v>-20.5</v>
       </c>
       <c r="H23">
         <v>-0.52</v>
@@ -1475,19 +1475,19 @@
         <v>35</v>
       </c>
       <c r="C24">
-        <v>-35.2</v>
+        <v>-29.6</v>
       </c>
       <c r="D24">
-        <v>-47.3</v>
+        <v>-34</v>
       </c>
       <c r="E24">
-        <v>-59.1</v>
+        <v>-26.6</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G24">
-        <v>-100</v>
+        <v>33</v>
       </c>
       <c r="H24">
         <v>-0.48</v>
@@ -1510,19 +1510,19 @@
         <v>36</v>
       </c>
       <c r="C25">
-        <v>-48.8</v>
+        <v>-45.2</v>
       </c>
       <c r="D25">
-        <v>-65</v>
+        <v>-56.8</v>
       </c>
       <c r="E25">
-        <v>-58.1</v>
+        <v>-42.3</v>
       </c>
       <c r="F25">
-        <v>2.6</v>
+        <v>62.6</v>
       </c>
       <c r="G25">
-        <v>-97</v>
+        <v>-26.4</v>
       </c>
       <c r="H25">
         <v>-1.11</v>
@@ -1545,19 +1545,19 @@
         <v>37</v>
       </c>
       <c r="C26">
-        <v>-34.5</v>
+        <v>-31.8</v>
       </c>
       <c r="D26">
-        <v>-48.1</v>
+        <v>-40.5</v>
       </c>
       <c r="E26">
-        <v>-43.5</v>
+        <v>-23.5</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>39.7</v>
       </c>
       <c r="G26">
-        <v>-100</v>
+        <v>-36</v>
       </c>
       <c r="H26">
         <v>-1.42</v>
@@ -1580,19 +1580,19 @@
         <v>38</v>
       </c>
       <c r="C27">
-        <v>-55.9</v>
+        <v>-52.8</v>
       </c>
       <c r="D27">
-        <v>-62.2</v>
+        <v>-53.8</v>
       </c>
       <c r="E27">
-        <v>-48</v>
+        <v>-28.6</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>55.7</v>
       </c>
       <c r="G27">
-        <v>-100</v>
+        <v>-40</v>
       </c>
       <c r="H27">
         <v>-1.28</v>
@@ -1615,19 +1615,19 @@
         <v>39</v>
       </c>
       <c r="C28">
-        <v>-18.7</v>
+        <v>-14.4</v>
       </c>
       <c r="D28">
-        <v>-30</v>
+        <v>-19.9</v>
       </c>
       <c r="E28">
-        <v>-38.4</v>
+        <v>-11.9</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="G28">
-        <v>-100</v>
+        <v>-3.3</v>
       </c>
       <c r="H28">
         <v>-0.54</v>
@@ -1659,19 +1659,19 @@
         <v>40</v>
       </c>
       <c r="C29">
-        <v>-50.2</v>
+        <v>-46.2</v>
       </c>
       <c r="D29">
-        <v>-61.3</v>
+        <v>-51.5</v>
       </c>
       <c r="E29">
-        <v>-36.2</v>
+        <v>-15.2</v>
       </c>
       <c r="F29">
-        <v>0.4</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="G29">
-        <v>-99.59999999999999</v>
+        <v>-34</v>
       </c>
       <c r="H29">
         <v>-0.43</v>
@@ -1692,7 +1692,7 @@
         <v>-36.83</v>
       </c>
       <c r="N29">
-        <v>-41.09</v>
+        <v>-34.39</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1703,19 +1703,19 @@
         <v>41</v>
       </c>
       <c r="C30">
-        <v>-12.2</v>
+        <v>-7.3</v>
       </c>
       <c r="D30">
-        <v>-13.2</v>
+        <v>-1</v>
       </c>
       <c r="E30">
-        <v>-1.6</v>
+        <v>31.5</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>89.40000000000001</v>
       </c>
       <c r="G30">
-        <v>-100</v>
+        <v>-12.1</v>
       </c>
       <c r="H30">
         <v>-0.71</v>
@@ -1747,19 +1747,19 @@
         <v>42</v>
       </c>
       <c r="C31">
-        <v>-22</v>
+        <v>-18.1</v>
       </c>
       <c r="D31">
-        <v>-31.6</v>
+        <v>-22.6</v>
       </c>
       <c r="E31">
-        <v>-42.3</v>
+        <v>-19</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>71.7</v>
       </c>
       <c r="G31">
-        <v>-100</v>
+        <v>-16.1</v>
       </c>
       <c r="H31">
         <v>-0.76</v>
@@ -1782,19 +1782,19 @@
         <v>43</v>
       </c>
       <c r="C32">
-        <v>-18.1</v>
+        <v>-14</v>
       </c>
       <c r="D32">
-        <v>-29.3</v>
+        <v>-19.7</v>
       </c>
       <c r="E32">
-        <v>-40</v>
+        <v>-15.2</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>71.2</v>
       </c>
       <c r="G32">
-        <v>-100</v>
+        <v>-7.5</v>
       </c>
       <c r="H32">
         <v>-0.54</v>
@@ -1826,19 +1826,19 @@
         <v>44</v>
       </c>
       <c r="C33">
-        <v>-36.4</v>
+        <v>-32.7</v>
       </c>
       <c r="D33">
-        <v>-41.4</v>
+        <v>-32.7</v>
       </c>
       <c r="E33">
-        <v>-42.3</v>
+        <v>-20.8</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>61.7</v>
       </c>
       <c r="G33">
-        <v>-100</v>
+        <v>-28.6</v>
       </c>
       <c r="H33">
         <v>-0.51</v>
@@ -1861,19 +1861,19 @@
         <v>45</v>
       </c>
       <c r="C34">
-        <v>-53.8</v>
+        <v>-50.8</v>
       </c>
       <c r="D34">
-        <v>-64.3</v>
+        <v>-57.1</v>
       </c>
       <c r="E34">
-        <v>-40</v>
+        <v>-23.7</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>47.2</v>
       </c>
       <c r="G34">
-        <v>-100</v>
+        <v>-31.8</v>
       </c>
       <c r="H34">
         <v>-0.49</v>
@@ -1894,7 +1894,7 @@
         <v>-21.07</v>
       </c>
       <c r="N34">
-        <v>-10.68</v>
+        <v>-11.59</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1905,19 +1905,19 @@
         <v>46</v>
       </c>
       <c r="C35">
-        <v>-57.8</v>
+        <v>-54.8</v>
       </c>
       <c r="D35">
-        <v>-63.2</v>
+        <v>-54.9</v>
       </c>
       <c r="E35">
-        <v>-48.8</v>
+        <v>-29.7</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G35">
-        <v>-100</v>
+        <v>-42.5</v>
       </c>
       <c r="H35">
         <v>-1.29</v>
@@ -1940,19 +1940,19 @@
         <v>47</v>
       </c>
       <c r="C36">
-        <v>-61</v>
+        <v>-59.4</v>
       </c>
       <c r="D36">
-        <v>-65.90000000000001</v>
+        <v>-61.9</v>
       </c>
       <c r="E36">
-        <v>-39.9</v>
+        <v>-30.6</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>31.2</v>
       </c>
       <c r="G36">
-        <v>-100</v>
+        <v>-70.09999999999999</v>
       </c>
       <c r="H36">
         <v>-0.43</v>
@@ -1973,7 +1973,7 @@
         <v>-78.25</v>
       </c>
       <c r="N36">
-        <v>-69.39</v>
+        <v>-70.86</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -1984,19 +1984,19 @@
         <v>48</v>
       </c>
       <c r="C37">
-        <v>-15.6</v>
+        <v>-11.3</v>
       </c>
       <c r="D37">
-        <v>-22.5</v>
+        <v>-12</v>
       </c>
       <c r="E37">
-        <v>-16.5</v>
+        <v>11.7</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="G37">
-        <v>-100</v>
+        <v>-15</v>
       </c>
       <c r="H37">
         <v>-0.64</v>
@@ -2028,19 +2028,19 @@
         <v>49</v>
       </c>
       <c r="C38">
-        <v>-47.3</v>
+        <v>-42.9</v>
       </c>
       <c r="D38">
-        <v>-63.7</v>
+        <v>-53.7</v>
       </c>
       <c r="E38">
-        <v>-50.7</v>
+        <v>-30.2</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>63.3</v>
       </c>
       <c r="G38">
-        <v>-100</v>
+        <v>-19.8</v>
       </c>
       <c r="H38">
         <v>-1.02</v>
@@ -2061,7 +2061,7 @@
         <v>-38.28</v>
       </c>
       <c r="N38">
-        <v>-43.58</v>
+        <v>-28.1</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2072,19 +2072,19 @@
         <v>50</v>
       </c>
       <c r="C39">
-        <v>-10.8</v>
+        <v>-5.6</v>
       </c>
       <c r="D39">
-        <v>-9.6</v>
+        <v>3.1</v>
       </c>
       <c r="E39">
-        <v>2.4</v>
+        <v>36.6</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>92.2</v>
       </c>
       <c r="G39">
-        <v>-100</v>
+        <v>-13.8</v>
       </c>
       <c r="H39">
         <v>-0.6899999999999999</v>
@@ -2116,19 +2116,19 @@
         <v>51</v>
       </c>
       <c r="C40">
-        <v>-17.7</v>
+        <v>-13.5</v>
       </c>
       <c r="D40">
-        <v>-28.1</v>
+        <v>-18.3</v>
       </c>
       <c r="E40">
-        <v>-26.9</v>
+        <v>-0.6</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="G40">
-        <v>-100</v>
+        <v>-12.7</v>
       </c>
       <c r="H40">
         <v>-0.63</v>
@@ -2160,19 +2160,19 @@
         <v>52</v>
       </c>
       <c r="C41">
-        <v>-52.4</v>
+        <v>-49.4</v>
       </c>
       <c r="D41">
-        <v>-61.2</v>
+        <v>-53.5</v>
       </c>
       <c r="E41">
-        <v>-44.3</v>
+        <v>-27.3</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>51.9</v>
       </c>
       <c r="G41">
-        <v>-100</v>
+        <v>-35.5</v>
       </c>
       <c r="H41">
         <v>-0.66</v>
@@ -2193,7 +2193,7 @@
         <v>-21.07</v>
       </c>
       <c r="N41">
-        <v>-10.68</v>
+        <v>-11.59</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2204,19 +2204,19 @@
         <v>53</v>
       </c>
       <c r="C42">
-        <v>-32.9</v>
+        <v>-26.8</v>
       </c>
       <c r="D42">
-        <v>-50.1</v>
+        <v>-36.3</v>
       </c>
       <c r="E42">
-        <v>-66.40000000000001</v>
+        <v>-34.2</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>101.3</v>
       </c>
       <c r="G42">
-        <v>-100</v>
+        <v>3.9</v>
       </c>
       <c r="H42">
         <v>-0.91</v>
@@ -2237,7 +2237,7 @@
         <v>-13.2</v>
       </c>
       <c r="N42">
-        <v>-14.94</v>
+        <v>-12.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>